<commit_message>
feat: actualizacion de fin de semana
</commit_message>
<xml_diff>
--- a/schema de horarios 2026.xlsx
+++ b/schema de horarios 2026.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11460" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Lunes-Viernes" sheetId="1" r:id="rId1"/>
@@ -165,10 +165,10 @@
     <t>Levantarte, lavarte los dientes, preparar café</t>
   </si>
   <si>
+    <t>6:55 – 7:15 am</t>
+  </si>
+  <si>
     <t>Lectura ligera (ficción, recreativa, inspiración suave)</t>
-  </si>
-  <si>
-    <t>6:55 – 7:15 am</t>
   </si>
   <si>
     <t>7:15 – 9:00 am</t>
@@ -409,7 +409,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -432,12 +432,6 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor theme="7" tint="0.599993896298105"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor theme="7" tint="0.799981688894314"/>
       </patternFill>
     </fill>
     <fill>
@@ -933,7 +927,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -957,16 +951,16 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -975,85 +969,85 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1097,10 +1091,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1112,10 +1106,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1859,7 +1853,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="57.1428571428571" defaultRowHeight="17" customHeight="1" outlineLevelCol="1"/>
@@ -1897,16 +1891,16 @@
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>45</v>
+      <c r="B4" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:2">
       <c r="A5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:2">

</xml_diff>